<commit_message>
se agrego la accion login, se modifico la clase execute y drivermanager.
</commit_message>
<xml_diff>
--- a/excel/GUI Automated Testing - Edit Profile.xlsx
+++ b/excel/GUI Automated Testing - Edit Profile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="GUI_EP_AP_001" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="76">
   <si>
     <t>Step</t>
   </si>
@@ -249,13 +249,16 @@
   </si>
   <si>
     <t>photopicker</t>
+  </si>
+  <si>
+    <t>(//mat-icon[@class='mat-icon notranslate material-icons mat-icon-no-color'])[5]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -311,6 +314,12 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -360,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -404,6 +413,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,8 +636,8 @@
   </sheetPr>
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1155,8 +1167,8 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1357,8 +1369,8 @@
       <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
+      <c r="F8" s="29" t="s">
+        <v>75</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -1380,7 +1392,7 @@
       <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="19" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="10"/>
@@ -1391,35 +1403,38 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="A10" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>74</v>
+        <v>14</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="A11" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="1" t="b">
+        <v>74</v>
+      </c>
+      <c r="I11" s="19" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="A12" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>14</v>
@@ -1439,7 +1454,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="A13" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>58</v>
@@ -1453,10 +1468,13 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>71</v>
+      </c>
+      <c r="I14" s="19" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1464,6 +1482,7 @@
     <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1472,10 +1491,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1890,10 +1909,21 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A19" s="27">
+      <c r="A19" s="11">
         <v>18</v>
       </c>
       <c r="B19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A20" s="11">
+        <v>19</v>
+      </c>
+      <c r="B20" s="28" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>